<commit_message>
fail to scan the invoice number
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -17,48 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;html xmlns="http://www.w3.org/1999/xhtml"&gt;
-    &lt;head&gt;
-        &lt;meta name="X-TIKA:Parsed-By" content="org.apache.tika.parser.EmptyParser"/&gt;
-        &lt;meta name="Content-Type" content="application/octet-stream"/&gt;
-        &lt;title&gt;&amp;#0;&lt;/title&gt;
-    &lt;/head&gt;
-    &lt;body/&gt;
-&lt;/html&gt;
-&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;html xmlns="http://www.w3.org/1999/xhtml"&gt;
-    &lt;head&gt;
-        &lt;meta name="pdf:PDFVersion" content="1.7"/&gt;
-        &lt;meta name="pdf:hasXFA" content="false"/&gt;
-        &lt;meta name="access_permission:modify_annotations" content="true"/&gt;
-        &lt;meta name="pdf:producer" content="iLovePDF"/&gt;
-        &lt;meta name="access_permission:can_print_degraded" content="true"/&gt;
-        &lt;meta name="access_permission:extract_for_accessibility" content="true"/&gt;
-        &lt;meta name="access_permission:assemble_document" content="true"/&gt;
-        &lt;meta name="xmpTPg:NPages" content="1"/&gt;
-        &lt;meta name="pdf:hasXMP" content="false"/&gt;
-        &lt;meta name="dcterms:modified" content="2023-03-03T07:34:00Z"/&gt;
-        &lt;meta name="dc:format" content="application/pdf; version=1.7"/&gt;
-        &lt;meta name="access_permission:extract_content" content="true"/&gt;
-        &lt;meta name="access_permission:can_print" content="true"/&gt;
-        &lt;meta name="access_permission:fill_in_form" content="true"/&gt;
-        &lt;meta name="pdf:docinfo:modified" content="2023-03-03T07:34:00Z"/&gt;
-        &lt;meta name="pdf:hasCollection" content="false"/&gt;
-        &lt;meta name="X-TIKA:Parsed-By" content="org.apache.tika.parser.DefaultParser"/&gt;
-        &lt;meta name="X-TIKA:Parsed-By" content="org.apache.tika.parser.pdf.PDFParser"/&gt;
-        &lt;meta name="pdf:encrypted" content="false"/&gt;
-        &lt;meta name="access_permission:can_modify" content="true"/&gt;
-        &lt;meta name="pdf:docinfo:producer" content="iLovePDF"/&gt;
-        &lt;meta name="pdf:hasMarkedContent" content="false"/&gt;
-        &lt;meta name="Content-Type" content="application/pdf"/&gt;
-        &lt;title&gt;&amp;#0;&lt;/title&gt;
-    &lt;/head&gt;
-    &lt;body&gt;
-        &lt;div class="page"&gt;
-            &lt;p/&gt;
-        &lt;/div&gt;
-    &lt;/body&gt;
-&lt;/html&gt;
-</t>
+    <t>&lt;p&gt;中国工商银行股份有限公司兰州中山支行2703050119200044428&lt;/p&gt;&lt;p&gt;兰州优行驰辰网络科技有限公司&lt;/p&gt;&lt;p&gt;91620100MA72R6U81E甘肃省兰州市安宁区北滨河西路530号连铝大厦19楼0931-8617788&lt;/p&gt;&lt;p&gt;招商银行兰州中央广场支行931905025010909&lt;/p&gt;&lt;p&gt;031/6&amp;gt;631-+/61**//7&amp;lt;/*101*02+1&amp;gt;9275+&amp;lt;6-615*981083&amp;gt;&amp;lt;7+3-&amp;gt;9491558-73&amp;lt;1-1816-98340298834-4/745*4-01&amp;gt;+78198-+/96301/&lt;/p&gt;&lt;p&gt;潘佳昕王玉平吴艳&lt;/p&gt;&lt;p&gt;*运输服务*客运服务费次1279.2279.20免税***&lt;/p&gt;&lt;p&gt;*运输服务*客运服务费-6.67免税***&lt;/p&gt;&lt;p&gt;¥272.53***&lt;/p&gt;&lt;p&gt;贰佰柒拾贰圆伍角叁分¥272.53&lt;/p&gt;</t>
   </si>
 </sst>
 </file>

</xml_diff>